<commit_message>
Still working on chapter 3
</commit_message>
<xml_diff>
--- a/admin_docs/PHC6099_topic_schedule_20240507.xlsx
+++ b/admin_docs/PHC6099_topic_schedule_20240507.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gabrielodom/Documents/GitHub/PHC6099_rBiostat/admin_docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A645D8A1-F088-914C-B6AE-8BF04408CFF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59004ACA-2CF4-5C46-8528-DD7AAA197C4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="89">
   <si>
     <t>Week</t>
   </si>
@@ -191,9 +191,6 @@
     <t>Dr. Odom at Conference</t>
   </si>
   <si>
-    <t>Power (Prof. Bursac)</t>
-  </si>
-  <si>
     <t>GLMs</t>
   </si>
   <si>
@@ -228,17 +225,100 @@
   </si>
   <si>
     <t>Bootstrap Tests</t>
+  </si>
+  <si>
+    <t>Machine Learning defense</t>
+  </si>
+  <si>
+    <t>Tarana Ferdous</t>
+  </si>
+  <si>
+    <t>Ivan Pachon</t>
+  </si>
+  <si>
+    <t>Gemma Galvez</t>
+  </si>
+  <si>
+    <t>Linear Mixed Effects</t>
+  </si>
+  <si>
+    <t>July</t>
+  </si>
+  <si>
+    <t>Structural Equation Modelling</t>
+  </si>
+  <si>
+    <t>Ekpereka Sandra Nawfal</t>
+  </si>
+  <si>
+    <t>Cox Proportional Hazards</t>
+  </si>
+  <si>
+    <t>Srijana Gautam</t>
+  </si>
+  <si>
+    <t>Freeman Lewis</t>
+  </si>
+  <si>
+    <t>TBD Multivariate + Genetics/Genomics</t>
+  </si>
+  <si>
+    <t>Ekpereka Sandra Nafwal</t>
+  </si>
+  <si>
+    <t>Ashlee Perez and Michaela Larson</t>
+  </si>
+  <si>
+    <t>(Prof. Bursac)</t>
+  </si>
+  <si>
+    <t>Power and Sample Size</t>
+  </si>
+  <si>
+    <t>Guillermo Rodriguez</t>
+  </si>
+  <si>
+    <t>Saurya Dhungel</t>
+  </si>
+  <si>
+    <t>Natalie Goulett</t>
+  </si>
+  <si>
+    <t>Melanie Freire</t>
+  </si>
+  <si>
+    <t>Noel Singh Dias and Jingwei Gu</t>
+  </si>
+  <si>
+    <t>Md Ariful Hoque</t>
+  </si>
+  <si>
+    <t>Elastic Net Regression</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -301,7 +381,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -344,8 +424,14 @@
         <bgColor rgb="FFDEEAF6"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -388,64 +474,162 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="15" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="15" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="15" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="15" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="15" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="15" fontId="4" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="15" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="15" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="15" fontId="4" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="15" fontId="4" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="15" fontId="2" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="15" fontId="4" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="15" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="15" fontId="2" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="15" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="15" fontId="2" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="15" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="15" fontId="2" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="15" fontId="4" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="15" fontId="4" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -693,10 +877,10 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -928,7 +1112,7 @@
         <v>45463</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
@@ -944,14 +1128,14 @@
         <v>45468</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E16" s="1"/>
       <c r="F16" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G16" s="21" t="s">
-        <v>57</v>
+      <c r="G16" s="17" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="17" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -965,14 +1149,14 @@
         <v>45470</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E17" s="1"/>
       <c r="F17" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G17" s="21" t="s">
-        <v>58</v>
+      <c r="G17" s="17" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="18" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -986,14 +1170,14 @@
         <v>45475</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E18" s="1"/>
       <c r="F18" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G18" s="21" t="s">
-        <v>61</v>
+      <c r="G18" s="17" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="19" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1043,14 +1227,14 @@
         <v>45482</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E20" s="1"/>
       <c r="F20" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G20" s="21" t="s">
-        <v>61</v>
+      <c r="G20" s="17" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="21" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1064,14 +1248,14 @@
         <v>45484</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E21" s="1"/>
       <c r="F21" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G21" s="21" t="s">
-        <v>61</v>
+      <c r="G21" s="17" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="22" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1085,14 +1269,14 @@
         <v>45489</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E22" s="1"/>
       <c r="F22" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G22" s="21" t="s">
-        <v>61</v>
+      <c r="G22" s="17" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="23" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1106,14 +1290,14 @@
         <v>45491</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E23" s="1"/>
       <c r="F23" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G23" s="21" t="s">
-        <v>61</v>
+      <c r="G23" s="17" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="24" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1127,14 +1311,14 @@
         <v>45496</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E24" s="1"/>
       <c r="F24" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G24" s="21" t="s">
-        <v>61</v>
+      <c r="G24" s="17" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="25" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2136,14 +2320,14 @@
   <dimension ref="A1:K1003"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.83203125" customWidth="1"/>
     <col min="2" max="2" width="32.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20" customWidth="1"/>
+    <col min="3" max="3" width="29.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" customWidth="1"/>
     <col min="5" max="5" width="44" customWidth="1"/>
     <col min="6" max="7" width="10.5" customWidth="1"/>
@@ -2160,7 +2344,7 @@
         <v>23</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="6"/>
@@ -2172,7 +2356,9 @@
       <c r="B2" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="9"/>
+      <c r="C2" s="9" t="s">
+        <v>79</v>
+      </c>
       <c r="E2" s="10"/>
     </row>
     <row r="3" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2182,126 +2368,130 @@
       <c r="B3" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="9"/>
-      <c r="E3" s="22"/>
+      <c r="C3" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="E3" s="18"/>
     </row>
     <row r="4" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="7">
+      <c r="A4" s="39">
         <v>45426</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="40" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="9"/>
+      <c r="C4" s="41"/>
       <c r="E4" s="10"/>
     </row>
     <row r="5" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="12">
+      <c r="A5" s="33"/>
+      <c r="B5" s="34"/>
+      <c r="C5" s="35"/>
+      <c r="E5" s="10"/>
+    </row>
+    <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="33">
         <v>45428</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B6" s="36" t="s">
+        <v>66</v>
+      </c>
+      <c r="C6" s="35"/>
+      <c r="E6" s="10"/>
+    </row>
+    <row r="7" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="33"/>
+      <c r="B7" s="34"/>
+      <c r="C7" s="35"/>
+      <c r="E7" s="10"/>
+    </row>
+    <row r="8" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="42">
+        <v>45433</v>
+      </c>
+      <c r="B8" s="44" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="14"/>
-      <c r="E5" s="10"/>
-    </row>
-    <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="12">
-        <v>45428</v>
-      </c>
-      <c r="B6" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="C6" s="14"/>
-      <c r="E6" s="10"/>
-    </row>
-    <row r="7" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="12">
-        <v>45428</v>
-      </c>
-      <c r="B7" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="C7" s="14"/>
-      <c r="E7" s="10"/>
-    </row>
-    <row r="8" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="7">
-        <v>45433</v>
-      </c>
-      <c r="B8" s="23" t="s">
-        <v>30</v>
-      </c>
-      <c r="C8" s="15"/>
+      <c r="C8" s="43"/>
     </row>
     <row r="9" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="7">
         <v>45433</v>
       </c>
-      <c r="B9" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="C9" s="9"/>
+      <c r="B9" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>85</v>
+      </c>
       <c r="E9" s="10"/>
     </row>
     <row r="10" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="7">
         <v>45433</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="E10" s="10"/>
+    </row>
+    <row r="11" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="19">
+        <v>45435</v>
+      </c>
+      <c r="B11" s="48" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="21"/>
+      <c r="E11" s="10"/>
+    </row>
+    <row r="12" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="11">
+        <v>45435</v>
+      </c>
+      <c r="B12" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="11">
+        <v>45435</v>
+      </c>
+      <c r="B13" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="9"/>
-      <c r="E10" s="10"/>
-    </row>
-    <row r="11" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="25">
-        <v>45435</v>
-      </c>
-      <c r="B11" s="26" t="s">
+      <c r="C13" s="13"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="10"/>
+    </row>
+    <row r="14" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="22">
+        <v>45440</v>
+      </c>
+      <c r="B14" s="45" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="27"/>
-      <c r="E11" s="10"/>
-    </row>
-    <row r="12" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="12">
-        <v>45435</v>
-      </c>
-      <c r="B12" s="24" t="s">
+      <c r="C14" s="23" t="s">
+        <v>76</v>
+      </c>
+      <c r="E14" s="10"/>
+    </row>
+    <row r="15" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="22">
+        <v>45440</v>
+      </c>
+      <c r="B15" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="16"/>
-    </row>
-    <row r="13" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="12">
-        <v>45435</v>
-      </c>
-      <c r="B13" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="C13" s="14"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="10"/>
-    </row>
-    <row r="14" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="28">
-        <v>45440</v>
-      </c>
-      <c r="B14" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="C14" s="30"/>
-      <c r="E14" s="10"/>
-    </row>
-    <row r="15" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="28">
-        <v>45440</v>
-      </c>
-      <c r="B15" s="31" t="s">
-        <v>66</v>
-      </c>
-      <c r="C15" s="30"/>
+      <c r="C15" s="9" t="s">
+        <v>79</v>
+      </c>
       <c r="E15" s="10"/>
       <c r="K15" s="10"/>
     </row>
@@ -2309,264 +2499,344 @@
       <c r="A16" s="7">
         <v>45440</v>
       </c>
-      <c r="B16" s="9" t="s">
+      <c r="B16" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="D16" s="14"/>
+      <c r="E16" s="10"/>
+    </row>
+    <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="19">
+        <v>45442</v>
+      </c>
+      <c r="B17" s="49" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" s="21"/>
+      <c r="E17" s="18"/>
+    </row>
+    <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="19">
+        <v>45442</v>
+      </c>
+      <c r="B18" s="50" t="s">
+        <v>65</v>
+      </c>
+      <c r="C18" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="E18" s="18"/>
+    </row>
+    <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="11">
+        <v>45442</v>
+      </c>
+      <c r="B19" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="C16" s="9"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="10"/>
-    </row>
-    <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="25">
-        <v>45442</v>
-      </c>
-      <c r="B17" s="27" t="s">
+      <c r="C19" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="E19" s="10"/>
+    </row>
+    <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="25">
+        <v>45447</v>
+      </c>
+      <c r="B20" s="47" t="s">
         <v>38</v>
       </c>
-      <c r="C17" s="27"/>
-      <c r="E17" s="22"/>
-    </row>
-    <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="25">
-        <v>45442</v>
-      </c>
-      <c r="B18" s="27" t="s">
+      <c r="C20" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="E20" s="1"/>
+    </row>
+    <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="25">
+        <v>45447</v>
+      </c>
+      <c r="B21" s="47" t="s">
         <v>39</v>
       </c>
-      <c r="C18" s="27"/>
-      <c r="E18" s="22"/>
-    </row>
-    <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="12">
-        <v>45442</v>
-      </c>
-      <c r="B19" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="C19" s="14"/>
-      <c r="E19" s="10"/>
-    </row>
-    <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="32">
-        <v>45447</v>
-      </c>
-      <c r="B20" s="30" t="s">
-        <v>41</v>
-      </c>
-      <c r="C20" s="30"/>
-      <c r="E20" s="1"/>
-    </row>
-    <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="32">
-        <v>45447</v>
-      </c>
-      <c r="B21" s="30" t="s">
-        <v>42</v>
-      </c>
-      <c r="C21" s="30"/>
+      <c r="C21" s="23" t="s">
+        <v>69</v>
+      </c>
       <c r="E21" s="1"/>
     </row>
     <row r="22" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="7">
         <v>45447</v>
       </c>
-      <c r="B22" s="8" t="s">
+      <c r="B22" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="C22" s="58"/>
+      <c r="E22" s="10"/>
+    </row>
+    <row r="23" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="11">
+        <v>45449</v>
+      </c>
+      <c r="B23" s="51" t="s">
+        <v>41</v>
+      </c>
+      <c r="C23" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="E23" s="10"/>
+    </row>
+    <row r="24" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="11">
+        <v>45449</v>
+      </c>
+      <c r="B24" s="51" t="s">
+        <v>42</v>
+      </c>
+      <c r="C24" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="E24" s="1"/>
+    </row>
+    <row r="25" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="11">
+        <v>45449</v>
+      </c>
+      <c r="B25" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="C22" s="9"/>
-      <c r="E22" s="10"/>
-    </row>
-    <row r="23" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="12">
-        <v>45449</v>
-      </c>
-      <c r="B23" s="26" t="s">
+      <c r="C25" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="E25" s="10"/>
+    </row>
+    <row r="26" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="22">
+        <v>45454</v>
+      </c>
+      <c r="B26" s="45" t="s">
         <v>44</v>
       </c>
-      <c r="C23" s="27"/>
-      <c r="E23" s="10"/>
-    </row>
-    <row r="24" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="12">
-        <v>45449</v>
-      </c>
-      <c r="B24" s="26" t="s">
+      <c r="C26" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="E26" s="10"/>
+    </row>
+    <row r="27" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="22">
+        <v>45454</v>
+      </c>
+      <c r="B27" s="45" t="s">
         <v>45</v>
       </c>
-      <c r="C24" s="27"/>
-      <c r="E24" s="1"/>
-    </row>
-    <row r="25" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="12">
-        <v>45449</v>
-      </c>
-      <c r="B25" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="C25" s="1"/>
-      <c r="E25" s="10"/>
-    </row>
-    <row r="26" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="28">
-        <v>45454</v>
-      </c>
-      <c r="B26" s="31" t="s">
-        <v>46</v>
-      </c>
-      <c r="C26" s="33"/>
-      <c r="E26" s="10"/>
-    </row>
-    <row r="27" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="28">
-        <v>45454</v>
-      </c>
-      <c r="B27" s="31" t="s">
-        <v>47</v>
-      </c>
-      <c r="C27" s="33"/>
-      <c r="D27" s="17"/>
+      <c r="C27" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="D27" s="14"/>
       <c r="E27" s="10"/>
     </row>
     <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="7">
         <v>45454</v>
       </c>
-      <c r="B28" s="8" t="s">
-        <v>48</v>
+      <c r="B28" s="24" t="s">
+        <v>62</v>
       </c>
       <c r="C28" s="9"/>
       <c r="E28" s="10"/>
     </row>
     <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="25">
+      <c r="A29" s="19">
         <v>45456</v>
       </c>
-      <c r="B29" s="26" t="s">
+      <c r="B29" s="50" t="s">
+        <v>46</v>
+      </c>
+      <c r="C29" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="E29" s="10"/>
+    </row>
+    <row r="30" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="19">
+        <v>45456</v>
+      </c>
+      <c r="B30" s="50" t="s">
+        <v>47</v>
+      </c>
+      <c r="C30" s="21"/>
+      <c r="D30" s="14"/>
+    </row>
+    <row r="31" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="11">
+        <v>45456</v>
+      </c>
+      <c r="B31" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="C31" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="E31" s="10"/>
+    </row>
+    <row r="32" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="11"/>
+      <c r="B32" s="12"/>
+      <c r="C32" s="13"/>
+      <c r="E32" s="10"/>
+    </row>
+    <row r="33" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="11">
+        <v>45461</v>
+      </c>
+      <c r="B33" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="C33" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="E33" s="10"/>
+    </row>
+    <row r="34" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="27"/>
+      <c r="B34" s="28"/>
+      <c r="C34" s="29"/>
+      <c r="E34" s="10"/>
+    </row>
+    <row r="35" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="37">
+        <v>45463</v>
+      </c>
+      <c r="B35" s="38" t="s">
         <v>49</v>
       </c>
-      <c r="C29" s="27"/>
-      <c r="E29" s="10"/>
-    </row>
-    <row r="30" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="25">
-        <v>45456</v>
-      </c>
-      <c r="B30" s="26" t="s">
+      <c r="C35" s="57" t="s">
+        <v>86</v>
+      </c>
+      <c r="E35" s="10"/>
+    </row>
+    <row r="36" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="37">
+        <v>45463</v>
+      </c>
+      <c r="B36" s="38" t="s">
         <v>50</v>
       </c>
-      <c r="C30" s="27"/>
-      <c r="D30" s="17"/>
-    </row>
-    <row r="31" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="12">
-        <v>45456</v>
-      </c>
-      <c r="B31" s="13" t="s">
+      <c r="C36" s="38" t="s">
+        <v>83</v>
+      </c>
+      <c r="D36" s="14"/>
+      <c r="E36" s="10"/>
+    </row>
+    <row r="37" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="37">
+        <v>45463</v>
+      </c>
+      <c r="B37" s="38" t="s">
         <v>51</v>
       </c>
-      <c r="C31" s="14"/>
-      <c r="E31" s="10"/>
-    </row>
-    <row r="32" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="12"/>
-      <c r="B32" s="13"/>
-      <c r="C32" s="14"/>
-      <c r="E32" s="10"/>
-    </row>
-    <row r="33" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="12">
-        <v>45461</v>
-      </c>
-      <c r="B33" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="C33" s="14"/>
-      <c r="E33" s="10"/>
-    </row>
-    <row r="34" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="12"/>
-      <c r="B34" s="13"/>
-      <c r="C34" s="14"/>
-      <c r="E34" s="10"/>
-    </row>
-    <row r="35" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="12">
-        <v>45463</v>
-      </c>
-      <c r="B35" s="13" t="s">
+      <c r="C37" s="57" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="30">
+        <v>45468</v>
+      </c>
+      <c r="B38" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="C35" s="14"/>
-      <c r="E35" s="10"/>
-    </row>
-    <row r="36" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="12">
-        <v>45463</v>
-      </c>
-      <c r="B36" s="18" t="s">
+      <c r="C38" s="32" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="11">
+        <v>45468</v>
+      </c>
+      <c r="B39" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="C39" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="D39" s="14"/>
+      <c r="E39" s="10"/>
+    </row>
+    <row r="40" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="11">
+        <v>45468</v>
+      </c>
+      <c r="B40" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="C36" s="14"/>
-      <c r="D36" s="17"/>
-      <c r="E36" s="10"/>
-    </row>
-    <row r="37" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="12">
-        <v>45463</v>
-      </c>
-      <c r="B37" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="C37" s="1"/>
-    </row>
-    <row r="38" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="19"/>
-      <c r="B38" s="14"/>
-      <c r="C38" s="20"/>
-    </row>
-    <row r="39" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="19"/>
-      <c r="B39" s="14"/>
-      <c r="C39" s="20"/>
-      <c r="D39" s="17"/>
-      <c r="E39" s="10"/>
-    </row>
-    <row r="40" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="19"/>
-      <c r="B40" s="14"/>
-      <c r="C40" s="20"/>
+      <c r="C40" s="16" t="s">
+        <v>84</v>
+      </c>
       <c r="E40" s="10"/>
     </row>
     <row r="41" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="19"/>
-      <c r="B41" s="14"/>
-      <c r="C41" s="20"/>
+      <c r="A41" s="52"/>
+      <c r="B41" s="29"/>
+      <c r="C41" s="53"/>
     </row>
     <row r="42" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="19"/>
-      <c r="B42" s="14"/>
-      <c r="C42" s="20"/>
+      <c r="A42" s="54" t="s">
+        <v>71</v>
+      </c>
+      <c r="B42" s="55" t="s">
+        <v>70</v>
+      </c>
+      <c r="C42" s="55" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="43" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="19"/>
-      <c r="B43" s="14"/>
-      <c r="C43" s="20"/>
+      <c r="A43" s="54" t="s">
+        <v>71</v>
+      </c>
+      <c r="B43" s="55" t="s">
+        <v>72</v>
+      </c>
+      <c r="C43" s="55" t="s">
+        <v>73</v>
+      </c>
       <c r="E43" s="10"/>
     </row>
     <row r="44" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="1"/>
-      <c r="B44" s="1"/>
-      <c r="C44" s="1"/>
+      <c r="A44" s="54" t="s">
+        <v>71</v>
+      </c>
+      <c r="B44" s="56" t="s">
+        <v>74</v>
+      </c>
+      <c r="C44" s="55" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="45" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="1"/>
-      <c r="B45" s="1"/>
-      <c r="C45" s="1"/>
+      <c r="A45" s="54" t="s">
+        <v>71</v>
+      </c>
+      <c r="B45" s="56" t="s">
+        <v>77</v>
+      </c>
+      <c r="C45" s="56" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="46" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="1"/>
-      <c r="B46" s="1"/>
-      <c r="C46" s="1"/>
+      <c r="A46" s="54" t="s">
+        <v>71</v>
+      </c>
+      <c r="B46" s="56" t="s">
+        <v>88</v>
+      </c>
+      <c r="C46" s="55" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="47" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="1"/>

</xml_diff>

<commit_message>
added lesson outline and example (one sample z-test) lesson
</commit_message>
<xml_diff>
--- a/admin_docs/PHC6099_topic_schedule_20240507.xlsx
+++ b/admin_docs/PHC6099_topic_schedule_20240507.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gabrielodom/Documents/GitHub/PHC6099_rBiostat/admin_docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59004ACA-2CF4-5C46-8528-DD7AAA197C4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60617909-EBC3-D740-A4EC-73D5DA02FF08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -542,7 +542,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="15" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -627,7 +627,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
@@ -2319,8 +2318,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K1003"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2503,7 +2502,7 @@
         <v>35</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D16" s="14"/>
       <c r="E16" s="10"/>
@@ -2573,7 +2572,7 @@
       <c r="B22" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="C22" s="58"/>
+      <c r="C22" s="57"/>
       <c r="E22" s="10"/>
     </row>
     <row r="23" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2596,7 +2595,7 @@
         <v>42</v>
       </c>
       <c r="C24" s="21" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E24" s="1"/>
     </row>
@@ -2712,7 +2711,7 @@
       <c r="B35" s="38" t="s">
         <v>49</v>
       </c>
-      <c r="C35" s="57" t="s">
+      <c r="C35" s="56" t="s">
         <v>86</v>
       </c>
       <c r="E35" s="10"/>
@@ -2737,7 +2736,7 @@
       <c r="B37" s="38" t="s">
         <v>51</v>
       </c>
-      <c r="C37" s="57" t="s">
+      <c r="C37" s="56" t="s">
         <v>86</v>
       </c>
     </row>
@@ -2809,7 +2808,7 @@
       <c r="A44" s="54" t="s">
         <v>71</v>
       </c>
-      <c r="B44" s="56" t="s">
+      <c r="B44" s="55" t="s">
         <v>74</v>
       </c>
       <c r="C44" s="55" t="s">
@@ -2820,10 +2819,10 @@
       <c r="A45" s="54" t="s">
         <v>71</v>
       </c>
-      <c r="B45" s="56" t="s">
+      <c r="B45" s="55" t="s">
         <v>77</v>
       </c>
-      <c r="C45" s="56" t="s">
+      <c r="C45" s="55" t="s">
         <v>76</v>
       </c>
     </row>
@@ -2831,7 +2830,7 @@
       <c r="A46" s="54" t="s">
         <v>71</v>
       </c>
-      <c r="B46" s="56" t="s">
+      <c r="B46" s="55" t="s">
         <v>88</v>
       </c>
       <c r="C46" s="55" t="s">

</xml_diff>

<commit_message>
adding Ashlee and Michaela's lessons
</commit_message>
<xml_diff>
--- a/admin_docs/PHC6099_topic_schedule_20240507.xlsx
+++ b/admin_docs/PHC6099_topic_schedule_20240507.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gabrielodom/Documents/GitHub/PHC6099_rBiostat/admin_docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7A4E8B2-678F-1D42-A78E-5E74547152FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CF0EC9F-EB3F-8C4E-AD2B-5DDD82247EF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="90">
   <si>
     <t>Week</t>
   </si>
@@ -240,9 +240,6 @@
   </si>
   <si>
     <t>Linear Mixed Effects</t>
-  </si>
-  <si>
-    <t>July</t>
   </si>
   <si>
     <t>Structural Equation Modelling</t>
@@ -306,7 +303,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -386,8 +383,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -436,8 +440,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -532,23 +548,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="15" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -596,10 +601,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="15" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="15" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
@@ -629,12 +630,21 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="15" fontId="4" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="15" fontId="4" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2322,10 +2332,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:K1004"/>
+  <dimension ref="A1:K1005"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2362,7 +2372,7 @@
         <v>24</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E2" s="10"/>
     </row>
@@ -2379,45 +2389,45 @@
       <c r="E3" s="18"/>
     </row>
     <row r="4" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="39">
+      <c r="A4" s="37">
         <v>45426</v>
       </c>
-      <c r="B4" s="40" t="s">
+      <c r="B4" s="38" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="41"/>
+      <c r="C4" s="39"/>
       <c r="E4" s="10"/>
     </row>
     <row r="5" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="33"/>
-      <c r="B5" s="34"/>
-      <c r="C5" s="35"/>
+      <c r="A5" s="31"/>
+      <c r="B5" s="32"/>
+      <c r="C5" s="33"/>
       <c r="E5" s="10"/>
     </row>
     <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="33">
+      <c r="A6" s="31">
         <v>45428</v>
       </c>
-      <c r="B6" s="36" t="s">
+      <c r="B6" s="34" t="s">
         <v>66</v>
       </c>
-      <c r="C6" s="35"/>
+      <c r="C6" s="33"/>
       <c r="E6" s="10"/>
     </row>
     <row r="7" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="33"/>
-      <c r="B7" s="34"/>
-      <c r="C7" s="35"/>
+      <c r="A7" s="31"/>
+      <c r="B7" s="32"/>
+      <c r="C7" s="33"/>
       <c r="E7" s="10"/>
     </row>
     <row r="8" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="42">
+      <c r="A8" s="40">
         <v>45433</v>
       </c>
-      <c r="B8" s="44" t="s">
+      <c r="B8" s="42" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="43"/>
+      <c r="C8" s="41"/>
     </row>
     <row r="9" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="7">
@@ -2427,7 +2437,7 @@
         <v>28</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E9" s="10"/>
     </row>
@@ -2447,7 +2457,7 @@
       <c r="A11" s="19">
         <v>45435</v>
       </c>
-      <c r="B11" s="48" t="s">
+      <c r="B11" s="46" t="s">
         <v>30</v>
       </c>
       <c r="C11" s="21"/>
@@ -2461,7 +2471,7 @@
         <v>31</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2479,11 +2489,11 @@
       <c r="A14" s="22">
         <v>45440</v>
       </c>
-      <c r="B14" s="45" t="s">
+      <c r="B14" s="43" t="s">
         <v>33</v>
       </c>
       <c r="C14" s="23" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E14" s="10"/>
     </row>
@@ -2491,11 +2501,11 @@
       <c r="A15" s="22">
         <v>45440</v>
       </c>
-      <c r="B15" s="46" t="s">
+      <c r="B15" s="44" t="s">
         <v>34</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E15" s="10"/>
       <c r="K15" s="10"/>
@@ -2508,7 +2518,7 @@
         <v>35</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D16" s="14"/>
       <c r="E16" s="10"/>
@@ -2517,7 +2527,7 @@
       <c r="A17" s="19">
         <v>45442</v>
       </c>
-      <c r="B17" s="49" t="s">
+      <c r="B17" s="47" t="s">
         <v>36</v>
       </c>
       <c r="C17" s="21"/>
@@ -2527,7 +2537,7 @@
       <c r="A18" s="19">
         <v>45442</v>
       </c>
-      <c r="B18" s="50" t="s">
+      <c r="B18" s="48" t="s">
         <v>65</v>
       </c>
       <c r="C18" s="21" t="s">
@@ -2543,7 +2553,7 @@
         <v>37</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E19" s="10"/>
     </row>
@@ -2551,11 +2561,11 @@
       <c r="A20" s="25">
         <v>45447</v>
       </c>
-      <c r="B20" s="47" t="s">
+      <c r="B20" s="45" t="s">
         <v>38</v>
       </c>
       <c r="C20" s="23" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E20" s="1"/>
     </row>
@@ -2563,7 +2573,7 @@
       <c r="A21" s="25">
         <v>45447</v>
       </c>
-      <c r="B21" s="47" t="s">
+      <c r="B21" s="45" t="s">
         <v>39</v>
       </c>
       <c r="C21" s="23" t="s">
@@ -2578,18 +2588,18 @@
       <c r="B22" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="C22" s="57"/>
+      <c r="C22" s="53"/>
       <c r="E22" s="10"/>
     </row>
     <row r="23" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="11">
         <v>45449</v>
       </c>
-      <c r="B23" s="51" t="s">
+      <c r="B23" s="49" t="s">
         <v>41</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E23" s="10"/>
     </row>
@@ -2597,11 +2607,11 @@
       <c r="A24" s="11">
         <v>45449</v>
       </c>
-      <c r="B24" s="51" t="s">
+      <c r="B24" s="49" t="s">
         <v>42</v>
       </c>
       <c r="C24" s="21" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E24" s="1"/>
     </row>
@@ -2613,7 +2623,7 @@
         <v>43</v>
       </c>
       <c r="C25" s="16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E25" s="10"/>
     </row>
@@ -2621,11 +2631,11 @@
       <c r="A26" s="22">
         <v>45454</v>
       </c>
-      <c r="B26" s="45" t="s">
+      <c r="B26" s="43" t="s">
         <v>44</v>
       </c>
       <c r="C26" s="23" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E26" s="10"/>
     </row>
@@ -2633,11 +2643,11 @@
       <c r="A27" s="22">
         <v>45454</v>
       </c>
-      <c r="B27" s="45" t="s">
+      <c r="B27" s="43" t="s">
         <v>45</v>
       </c>
       <c r="C27" s="26" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D27" s="14"/>
       <c r="E27" s="10"/>
@@ -2656,11 +2666,11 @@
       <c r="A29" s="19">
         <v>45456</v>
       </c>
-      <c r="B29" s="50" t="s">
+      <c r="B29" s="48" t="s">
         <v>46</v>
       </c>
       <c r="C29" s="21" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E29" s="10"/>
     </row>
@@ -2668,7 +2678,7 @@
       <c r="A30" s="19">
         <v>45456</v>
       </c>
-      <c r="B30" s="50" t="s">
+      <c r="B30" s="48" t="s">
         <v>47</v>
       </c>
       <c r="C30" s="21"/>
@@ -2682,7 +2692,7 @@
         <v>48</v>
       </c>
       <c r="C31" s="13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E31" s="10"/>
     </row>
@@ -2693,26 +2703,26 @@
       <c r="E32" s="10"/>
     </row>
     <row r="33" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="11">
+      <c r="A33" s="54">
         <v>45461</v>
       </c>
-      <c r="B33" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="C33" s="13" t="s">
+      <c r="B33" s="55" t="s">
         <v>80</v>
       </c>
+      <c r="C33" s="56" t="s">
+        <v>79</v>
+      </c>
       <c r="E33" s="10"/>
     </row>
     <row r="34" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="11">
+      <c r="A34" s="54">
         <v>45463</v>
       </c>
-      <c r="B34" s="12" t="s">
+      <c r="B34" s="55" t="s">
+        <v>88</v>
+      </c>
+      <c r="C34" s="56" t="s">
         <v>89</v>
-      </c>
-      <c r="C34" s="13" t="s">
-        <v>90</v>
       </c>
       <c r="E34" s="10"/>
     </row>
@@ -2723,51 +2733,43 @@
       <c r="E35" s="10"/>
     </row>
     <row r="36" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="37">
+      <c r="A36" s="35">
         <v>45468</v>
       </c>
-      <c r="B36" s="38" t="s">
+      <c r="B36" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="C36" s="56" t="s">
-        <v>86</v>
+      <c r="C36" s="52" t="s">
+        <v>85</v>
       </c>
       <c r="E36" s="10"/>
     </row>
     <row r="37" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="37">
+      <c r="A37" s="35">
         <v>45468</v>
       </c>
-      <c r="B37" s="38" t="s">
+      <c r="B37" s="36" t="s">
         <v>50</v>
       </c>
-      <c r="C37" s="38" t="s">
-        <v>83</v>
+      <c r="C37" s="36" t="s">
+        <v>82</v>
       </c>
       <c r="D37" s="14"/>
       <c r="E37" s="10"/>
     </row>
     <row r="38" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="37">
+      <c r="A38" s="35">
         <v>45468</v>
       </c>
-      <c r="B38" s="38" t="s">
+      <c r="B38" s="36" t="s">
         <v>51</v>
       </c>
-      <c r="C38" s="56" t="s">
-        <v>86</v>
+      <c r="C38" s="52" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="30">
-        <v>45470</v>
-      </c>
-      <c r="B39" s="31" t="s">
-        <v>52</v>
-      </c>
-      <c r="C39" s="32" t="s">
-        <v>69</v>
-      </c>
+      <c r="A39" s="30"/>
     </row>
     <row r="40" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="11">
@@ -2777,88 +2779,94 @@
         <v>63</v>
       </c>
       <c r="C40" s="16" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D40" s="14"/>
       <c r="E40" s="10"/>
     </row>
     <row r="41" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="11">
-        <v>45470</v>
-      </c>
-      <c r="B41" s="12" t="s">
+      <c r="A41" s="57">
+        <v>45475</v>
+      </c>
+      <c r="B41" s="58" t="s">
+        <v>52</v>
+      </c>
+      <c r="C41" s="59" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="50"/>
+      <c r="B42" s="51"/>
+      <c r="C42" s="51"/>
+    </row>
+    <row r="43" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="50">
+        <v>45482</v>
+      </c>
+      <c r="B43" s="51" t="s">
+        <v>87</v>
+      </c>
+      <c r="C43" s="51" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="50">
+        <v>45484</v>
+      </c>
+      <c r="B44" s="51" t="s">
+        <v>73</v>
+      </c>
+      <c r="C44" s="51" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="50">
+        <v>45489</v>
+      </c>
+      <c r="B45" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="C41" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="E41" s="10"/>
-    </row>
-    <row r="42" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="52"/>
-      <c r="B42" s="29"/>
-      <c r="C42" s="53"/>
-    </row>
-    <row r="43" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="54" t="s">
+      <c r="C45" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="E45" s="10"/>
+    </row>
+    <row r="46" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="50">
+        <v>45491</v>
+      </c>
+      <c r="B46" s="51" t="s">
+        <v>70</v>
+      </c>
+      <c r="C46" s="51" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="50">
+        <v>45496</v>
+      </c>
+      <c r="B47" s="51" t="s">
         <v>71</v>
       </c>
-      <c r="B43" s="55" t="s">
-        <v>70</v>
-      </c>
-      <c r="C43" s="55" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="54" t="s">
-        <v>71</v>
-      </c>
-      <c r="B44" s="55" t="s">
+      <c r="C47" s="51" t="s">
         <v>72</v>
       </c>
-      <c r="C44" s="55" t="s">
-        <v>73</v>
-      </c>
-      <c r="E44" s="10"/>
-    </row>
-    <row r="45" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="54" t="s">
-        <v>71</v>
-      </c>
-      <c r="B45" s="55" t="s">
-        <v>74</v>
-      </c>
-      <c r="C45" s="55" t="s">
+      <c r="E47" s="10"/>
+    </row>
+    <row r="48" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="60">
+        <v>45498</v>
+      </c>
+      <c r="B48" s="51" t="s">
+        <v>76</v>
+      </c>
+      <c r="C48" s="51" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="54" t="s">
-        <v>71</v>
-      </c>
-      <c r="B46" s="55" t="s">
-        <v>77</v>
-      </c>
-      <c r="C46" s="55" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="54" t="s">
-        <v>71</v>
-      </c>
-      <c r="B47" s="55" t="s">
-        <v>88</v>
-      </c>
-      <c r="C47" s="55" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="1"/>
-      <c r="B48" s="1"/>
-      <c r="C48" s="1"/>
     </row>
     <row r="49" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="1"/>
@@ -7639,6 +7647,11 @@
       <c r="A1004" s="1"/>
       <c r="B1004" s="1"/>
       <c r="C1004" s="1"/>
+    </row>
+    <row r="1005" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1005" s="1"/>
+      <c r="B1005" s="1"/>
+      <c r="C1005" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>

</xml_diff>